<commit_message>
màj backlog toutes les tâches
</commit_message>
<xml_diff>
--- a/suivi.xlsx
+++ b/suivi.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t>Installer python3, python3-pip, python3-dev, git, visual studio code</t>
   </si>
@@ -38,9 +38,6 @@
     <t>Cloner dans home : https://github.com/vanessakovalsky/example-python.git</t>
   </si>
   <si>
-    <t>backlog postes dèv</t>
-  </si>
-  <si>
     <t>Vérifier que la VM démarre avec un vagrant up</t>
   </si>
   <si>
@@ -78,13 +75,103 @@
   </si>
   <si>
     <t>Enzo</t>
+  </si>
+  <si>
+    <t>backlog</t>
+  </si>
+  <si>
+    <t>Postes de développement</t>
+  </si>
+  <si>
+    <t>Serveur Web</t>
+  </si>
+  <si>
+    <t>Installer apache2</t>
+  </si>
+  <si>
+    <t>Vérifier que le service tourne (ou faire sa configuration)</t>
+  </si>
+  <si>
+    <t>Changer récursivement le groupe de /var/www/html par le groupe www-data (lecture/écriture)</t>
+  </si>
+  <si>
+    <t>Dans /var/www/html : créer la page index.html (selon indications de l'énoncé)</t>
+  </si>
+  <si>
+    <t>Installer un pare-feu (genre UFW)</t>
+  </si>
+  <si>
+    <t>Tester installation du paquet (manuellement)</t>
+  </si>
+  <si>
+    <t>Ouvrir les ports 80 et 443 via le-dit pare-feu</t>
+  </si>
+  <si>
+    <t>Vérifier l'accès à la page web (manuellement)</t>
+  </si>
+  <si>
+    <t>Serveur Jenkins</t>
+  </si>
+  <si>
+    <t>création partition sur le disque 2 (ext4)</t>
+  </si>
+  <si>
+    <t>installation de Jenkins et ses dépendances</t>
+  </si>
+  <si>
+    <t>Démarrer le service (configurer pour démarrage automatique)</t>
+  </si>
+  <si>
+    <t>Créer l'utilisateur userjob</t>
+  </si>
+  <si>
+    <t>Lui donner le droit d'utiliser apt dans le fichier sudoers</t>
+  </si>
+  <si>
+    <t>Afficher le contenu de /var/jenkins_home/secrets/initialAdminPassword</t>
+  </si>
+  <si>
+    <t>Ouvrir les ports de Jenkins et le port 22</t>
+  </si>
+  <si>
+    <t>Vérifier la connexion à Jenkins en web (manuellement)</t>
+  </si>
+  <si>
+    <t>Vérifier la connexion en SSH depuis les postes de développement (manuellement)</t>
+  </si>
+  <si>
+    <t>Vérifier la présence du client NFS (manuellement)</t>
+  </si>
+  <si>
+    <t>Vérifier la présence de rsync (manuellement)</t>
+  </si>
+  <si>
+    <t>Créer un point de montage permanent vers le serveur NFS</t>
+  </si>
+  <si>
+    <t>Créer une tâche cron qui sauvegarde /var/www/html sur le NFS (dossier web, voir énoncé)</t>
+  </si>
+  <si>
+    <t>Créer une tâche cron qui sauvegarde /usr/local/jenkins sur le NFS (dossier server_ic, voir énoncé)</t>
+  </si>
+  <si>
+    <t>Serveur NFS</t>
+  </si>
+  <si>
+    <t>Installer le serveur NFS</t>
+  </si>
+  <si>
+    <t>Créer les dossiers partagés : web et server_ic (voir énoncé)</t>
+  </si>
+  <si>
+    <t>créer une tâche cron pour la rétention de 7 jours des sauvegardes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,8 +179,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -118,8 +213,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -127,17 +228,223 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E29"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -432,109 +739,403 @@
     <col min="5" max="5" width="38.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="10"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B11" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+      <c r="C11" s="9"/>
+      <c r="D11" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="10"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="10"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
+      <c r="C14" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="10"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+      <c r="D15" s="9"/>
+      <c r="E15" s="10"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B16" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B23" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="10"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B25" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="10"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B26" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="10"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B27" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="10"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B28" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="21"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B29" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="10"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B30" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="10"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B31" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="10"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B32" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="10"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B33" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="10"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B34" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="10"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B35" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="10"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B36" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="10"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B37" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="10"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B38" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="10"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B39" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="10"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B40" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="10"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B41" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="10"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B42" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="10"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B43" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="21"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B44" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="10"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B45" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="10"/>
+    </row>
+    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="17"/>
+    </row>
+    <row r="47" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B28" s="2" t="s">
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B29" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C43:E43"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
modification v.1 du suivi
</commit_message>
<xml_diff>
--- a/suivi.xlsx
+++ b/suivi.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ib\Documents\TP_linux_avril\Tp - Linux - Avril\scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ib\Desktop\Linux-Avril\Rendu-TP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9528"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -179,7 +179,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -489,6 +489,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -501,11 +506,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -788,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -819,9 +819,9 @@
       <c r="B3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="21"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="26"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
@@ -933,52 +933,52 @@
       <c r="B16" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="23"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="28"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="26"/>
+      <c r="C17" s="22"/>
       <c r="D17" s="9"/>
       <c r="E17" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="26"/>
+      <c r="C18" s="22"/>
       <c r="D18" s="9"/>
       <c r="E18" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="26"/>
+      <c r="C19" s="22"/>
       <c r="D19" s="9"/>
       <c r="E19" s="12" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="26"/>
+      <c r="C20" s="22"/>
       <c r="D20" s="9"/>
       <c r="E20" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="9"/>
@@ -988,7 +988,7 @@
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="21" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="9"/>
@@ -1012,7 +1012,7 @@
         <v>38</v>
       </c>
       <c r="C24" s="9"/>
-      <c r="D24" s="24"/>
+      <c r="D24" s="20"/>
       <c r="E24" s="12" t="s">
         <v>38</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>39</v>
       </c>
       <c r="C25" s="9"/>
-      <c r="D25" s="24"/>
+      <c r="D25" s="20"/>
       <c r="E25" s="12" t="s">
         <v>39</v>
       </c>
@@ -1047,16 +1047,16 @@
       <c r="B28" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="23"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="28"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C29" s="9"/>
-      <c r="D29" s="27"/>
+      <c r="D29" s="23"/>
       <c r="E29" s="19" t="s">
         <v>29</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>30</v>
       </c>
       <c r="C30" s="9"/>
-      <c r="D30" s="27"/>
+      <c r="D30" s="23"/>
       <c r="E30" s="19" t="s">
         <v>30</v>
       </c>
@@ -1076,43 +1076,40 @@
         <v>31</v>
       </c>
       <c r="C31" s="9"/>
-      <c r="D31" s="27"/>
+      <c r="D31" s="23"/>
       <c r="E31" s="19" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B32" s="25" t="s">
+      <c r="B32" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="D32" s="9"/>
+      <c r="E32" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="9"/>
-      <c r="E32" s="10"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B33" s="25" t="s">
+      <c r="B33" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="D33" s="9"/>
+      <c r="E33" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="9"/>
-      <c r="E33" s="10"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B34" s="25" t="s">
+      <c r="B34" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="D34" s="9"/>
+      <c r="E34" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="9"/>
-      <c r="E34" s="10"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B35" s="25" t="s">
+      <c r="B35" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C35" s="8" t="s">
@@ -1122,14 +1119,13 @@
       <c r="E35" s="10"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B36" s="25" t="s">
+      <c r="B36" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="D36" s="9"/>
+      <c r="E36" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="9"/>
-      <c r="E36" s="10"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B37" s="7" t="s">
@@ -1183,9 +1179,9 @@
       <c r="B43" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="23"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="28"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B44" s="14" t="s">
@@ -1211,7 +1207,7 @@
       <c r="B46" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C46" s="28" t="s">
+      <c r="C46" s="24" t="s">
         <v>49</v>
       </c>
       <c r="D46" s="16"/>

</xml_diff>

<commit_message>
modification v.2 du suivi
</commit_message>
<xml_diff>
--- a/suivi.xlsx
+++ b/suivi.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
   <si>
     <t>Installer python3, python3-pip, python3-dev, git, visual studio code</t>
   </si>
@@ -458,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -506,6 +506,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -789,7 +790,7 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1131,7 +1132,9 @@
       <c r="B37" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="9"/>
+      <c r="C37" s="29" t="s">
+        <v>36</v>
+      </c>
       <c r="D37" s="9"/>
       <c r="E37" s="10"/>
     </row>
@@ -1139,7 +1142,9 @@
       <c r="B38" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="9"/>
+      <c r="C38" s="29" t="s">
+        <v>37</v>
+      </c>
       <c r="D38" s="9"/>
       <c r="E38" s="10"/>
     </row>
@@ -1147,7 +1152,9 @@
       <c r="B39" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="9"/>
+      <c r="C39" s="29" t="s">
+        <v>38</v>
+      </c>
       <c r="D39" s="9"/>
       <c r="E39" s="10"/>
     </row>
@@ -1155,7 +1162,9 @@
       <c r="B40" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="9"/>
+      <c r="C40" s="29" t="s">
+        <v>39</v>
+      </c>
       <c r="D40" s="9"/>
       <c r="E40" s="10"/>
     </row>

</xml_diff>

<commit_message>
modification v.3 du suivi
</commit_message>
<xml_diff>
--- a/suivi.xlsx
+++ b/suivi.xlsx
@@ -494,6 +494,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -506,7 +507,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -789,7 +789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
@@ -820,9 +820,9 @@
       <c r="B3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
@@ -934,9 +934,9 @@
       <c r="B16" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="29"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="21" t="s">
@@ -1048,9 +1048,9 @@
       <c r="B28" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="29"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="7" t="s">
@@ -1132,7 +1132,7 @@
       <c r="B37" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="29" t="s">
+      <c r="C37" s="25" t="s">
         <v>36</v>
       </c>
       <c r="D37" s="9"/>
@@ -1142,7 +1142,7 @@
       <c r="B38" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="29" t="s">
+      <c r="C38" s="25" t="s">
         <v>37</v>
       </c>
       <c r="D38" s="9"/>
@@ -1152,7 +1152,7 @@
       <c r="B39" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="29" t="s">
+      <c r="C39" s="25" t="s">
         <v>38</v>
       </c>
       <c r="D39" s="9"/>
@@ -1162,7 +1162,7 @@
       <c r="B40" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="29" t="s">
+      <c r="C40" s="25" t="s">
         <v>39</v>
       </c>
       <c r="D40" s="9"/>
@@ -1188,9 +1188,9 @@
       <c r="B43" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="28"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="29"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B44" s="14" t="s">

</xml_diff>

<commit_message>
modification v 3.3 suivi
</commit_message>
<xml_diff>
--- a/suivi.xlsx
+++ b/suivi.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="54">
   <si>
     <t>Installer python3, python3-pip, python3-dev, git, visual studio code</t>
   </si>
@@ -801,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -850,7 +850,9 @@
       <c r="B5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="9"/>
+      <c r="C5" s="25" t="s">
+        <v>1</v>
+      </c>
       <c r="D5" s="9"/>
       <c r="E5" s="10"/>
     </row>
@@ -858,7 +860,9 @@
       <c r="B6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="9"/>
+      <c r="C6" s="25" t="s">
+        <v>2</v>
+      </c>
       <c r="D6" s="9"/>
       <c r="E6" s="10"/>
     </row>
@@ -866,7 +870,9 @@
       <c r="B7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="9"/>
+      <c r="C7" s="25" t="s">
+        <v>3</v>
+      </c>
       <c r="D7" s="9"/>
       <c r="E7" s="10"/>
     </row>
@@ -874,7 +880,9 @@
       <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="9"/>
+      <c r="C8" s="25" t="s">
+        <v>4</v>
+      </c>
       <c r="D8" s="9"/>
       <c r="E8" s="10"/>
     </row>
@@ -882,7 +890,9 @@
       <c r="B9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="9"/>
+      <c r="C9" s="25" t="s">
+        <v>5</v>
+      </c>
       <c r="D9" s="9"/>
       <c r="E9" s="10"/>
     </row>
@@ -890,7 +900,9 @@
       <c r="B10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="9"/>
+      <c r="C10" s="25" t="s">
+        <v>6</v>
+      </c>
       <c r="D10" s="9"/>
       <c r="E10" s="10"/>
     </row>

</xml_diff>

<commit_message>
màj des tâches du jour
</commit_message>
<xml_diff>
--- a/suivi.xlsx
+++ b/suivi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ib\Desktop\Linux-Avril\Rendu-TP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ib\Documents\TP_linux_avril\Tp - Linux - Avril\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -191,7 +191,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -498,14 +498,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -519,6 +517,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -801,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44:D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -832,17 +832,17 @@
       <c r="B3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="27"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="18"/>
+      <c r="C4" s="17"/>
       <c r="D4" s="9"/>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="18" t="s">
         <v>0</v>
       </c>
     </row>
@@ -850,7 +850,7 @@
       <c r="B5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="23" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="9"/>
@@ -860,7 +860,7 @@
       <c r="B6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="23" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="9"/>
@@ -870,7 +870,7 @@
       <c r="B7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="23" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="9"/>
@@ -880,7 +880,7 @@
       <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="23" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="9"/>
@@ -890,7 +890,7 @@
       <c r="B9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="23" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="9"/>
@@ -900,7 +900,7 @@
       <c r="B10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="23" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="9"/>
@@ -938,7 +938,7 @@
       <c r="B14" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="18"/>
+      <c r="C14" s="17"/>
       <c r="D14" s="8" t="s">
         <v>7</v>
       </c>
@@ -958,52 +958,52 @@
       <c r="B16" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="29"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="27"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="22"/>
+      <c r="C17" s="21"/>
       <c r="D17" s="9"/>
       <c r="E17" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="22"/>
+      <c r="C18" s="21"/>
       <c r="D18" s="9"/>
       <c r="E18" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="22"/>
+      <c r="C19" s="21"/>
       <c r="D19" s="9"/>
       <c r="E19" s="12" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="22"/>
+      <c r="C20" s="21"/>
       <c r="D20" s="9"/>
       <c r="E20" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="20" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="9"/>
@@ -1013,7 +1013,7 @@
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="20" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="9"/>
@@ -1037,7 +1037,7 @@
         <v>38</v>
       </c>
       <c r="C24" s="9"/>
-      <c r="D24" s="20"/>
+      <c r="D24" s="19"/>
       <c r="E24" s="12" t="s">
         <v>38</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>39</v>
       </c>
       <c r="C25" s="9"/>
-      <c r="D25" s="20"/>
+      <c r="D25" s="19"/>
       <c r="E25" s="12" t="s">
         <v>39</v>
       </c>
@@ -1056,37 +1056,37 @@
       <c r="B26" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="10"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="10"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="29"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="27"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C29" s="9"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="19" t="s">
+      <c r="D29" s="22"/>
+      <c r="E29" s="18" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1095,8 +1095,8 @@
         <v>30</v>
       </c>
       <c r="C30" s="9"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="19" t="s">
+      <c r="D30" s="22"/>
+      <c r="E30" s="18" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1105,13 +1105,13 @@
         <v>31</v>
       </c>
       <c r="C31" s="9"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="19" t="s">
+      <c r="D31" s="22"/>
+      <c r="E31" s="18" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="20" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="9"/>
@@ -1121,7 +1121,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="20" t="s">
         <v>32</v>
       </c>
       <c r="C33" s="9"/>
@@ -1131,7 +1131,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B34" s="21" t="s">
+      <c r="B34" s="20" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="9"/>
@@ -1141,7 +1141,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="20" t="s">
         <v>24</v>
       </c>
       <c r="D35" s="9"/>
@@ -1150,7 +1150,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D36" s="9"/>
@@ -1163,7 +1163,7 @@
         <v>36</v>
       </c>
       <c r="D37" s="9"/>
-      <c r="E37" s="25" t="s">
+      <c r="E37" s="23" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
         <v>37</v>
       </c>
       <c r="D38" s="9"/>
-      <c r="E38" s="25" t="s">
+      <c r="E38" s="23" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1180,7 +1180,7 @@
       <c r="B39" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="25" t="s">
+      <c r="C39" s="23" t="s">
         <v>38</v>
       </c>
       <c r="D39" s="9"/>
@@ -1190,7 +1190,7 @@
       <c r="B40" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="25" t="s">
+      <c r="C40" s="23" t="s">
         <v>39</v>
       </c>
       <c r="D40" s="9"/>
@@ -1200,59 +1200,59 @@
       <c r="B41" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="9"/>
-      <c r="E41" s="10"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B42" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="D42" s="9"/>
-      <c r="E42" s="10"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B43" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="29"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="27"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B44" s="14" t="s">
         <v>44</v>
       </c>
       <c r="C44" s="9"/>
-      <c r="D44" s="11" t="s">
+      <c r="D44" s="21"/>
+      <c r="E44" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E44" s="10"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B45" s="14" t="s">
         <v>45</v>
       </c>
       <c r="C45" s="9"/>
-      <c r="D45" s="11" t="s">
+      <c r="D45" s="21"/>
+      <c r="E45" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="E45" s="10"/>
     </row>
     <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B46" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C46" s="24" t="s">
+      <c r="C46" s="29"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="D46" s="16"/>
-      <c r="E46" s="17"/>
     </row>
     <row r="47" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
modification v 4.4 suivi et install vagrant
</commit_message>
<xml_diff>
--- a/suivi.xlsx
+++ b/suivi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ib\Desktop\Linux-Avril\Rendu-TP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ib\Documents\TP_linux_avril\Tp - Linux - Avril\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -191,7 +191,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -498,14 +498,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -519,6 +517,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -801,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44:D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -832,17 +832,17 @@
       <c r="B3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="27"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="18"/>
+      <c r="C4" s="17"/>
       <c r="D4" s="9"/>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="18" t="s">
         <v>0</v>
       </c>
     </row>
@@ -850,7 +850,7 @@
       <c r="B5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="23" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="9"/>
@@ -860,7 +860,7 @@
       <c r="B6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="23" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="9"/>
@@ -870,7 +870,7 @@
       <c r="B7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="23" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="9"/>
@@ -880,7 +880,7 @@
       <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="23" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="9"/>
@@ -890,7 +890,7 @@
       <c r="B9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="23" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="9"/>
@@ -900,7 +900,7 @@
       <c r="B10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="23" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="9"/>
@@ -938,7 +938,7 @@
       <c r="B14" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="18"/>
+      <c r="C14" s="17"/>
       <c r="D14" s="8" t="s">
         <v>7</v>
       </c>
@@ -958,52 +958,52 @@
       <c r="B16" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="29"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="27"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="22"/>
+      <c r="C17" s="21"/>
       <c r="D17" s="9"/>
       <c r="E17" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="22"/>
+      <c r="C18" s="21"/>
       <c r="D18" s="9"/>
       <c r="E18" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="22"/>
+      <c r="C19" s="21"/>
       <c r="D19" s="9"/>
       <c r="E19" s="12" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="22"/>
+      <c r="C20" s="21"/>
       <c r="D20" s="9"/>
       <c r="E20" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="20" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="9"/>
@@ -1013,7 +1013,7 @@
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="20" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="9"/>
@@ -1037,7 +1037,7 @@
         <v>38</v>
       </c>
       <c r="C24" s="9"/>
-      <c r="D24" s="20"/>
+      <c r="D24" s="19"/>
       <c r="E24" s="12" t="s">
         <v>38</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>39</v>
       </c>
       <c r="C25" s="9"/>
-      <c r="D25" s="20"/>
+      <c r="D25" s="19"/>
       <c r="E25" s="12" t="s">
         <v>39</v>
       </c>
@@ -1056,37 +1056,37 @@
       <c r="B26" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="10"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="10"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="29"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="27"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C29" s="9"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="19" t="s">
+      <c r="D29" s="22"/>
+      <c r="E29" s="18" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1095,8 +1095,8 @@
         <v>30</v>
       </c>
       <c r="C30" s="9"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="19" t="s">
+      <c r="D30" s="22"/>
+      <c r="E30" s="18" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1105,13 +1105,13 @@
         <v>31</v>
       </c>
       <c r="C31" s="9"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="19" t="s">
+      <c r="D31" s="22"/>
+      <c r="E31" s="18" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="20" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="9"/>
@@ -1121,7 +1121,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="20" t="s">
         <v>32</v>
       </c>
       <c r="C33" s="9"/>
@@ -1131,7 +1131,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B34" s="21" t="s">
+      <c r="B34" s="20" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="9"/>
@@ -1141,7 +1141,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="20" t="s">
         <v>24</v>
       </c>
       <c r="D35" s="9"/>
@@ -1150,7 +1150,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D36" s="9"/>
@@ -1163,7 +1163,7 @@
         <v>36</v>
       </c>
       <c r="D37" s="9"/>
-      <c r="E37" s="25" t="s">
+      <c r="E37" s="23" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
         <v>37</v>
       </c>
       <c r="D38" s="9"/>
-      <c r="E38" s="25" t="s">
+      <c r="E38" s="23" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1180,7 +1180,7 @@
       <c r="B39" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="25" t="s">
+      <c r="C39" s="23" t="s">
         <v>38</v>
       </c>
       <c r="D39" s="9"/>
@@ -1190,7 +1190,7 @@
       <c r="B40" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="25" t="s">
+      <c r="C40" s="23" t="s">
         <v>39</v>
       </c>
       <c r="D40" s="9"/>
@@ -1200,59 +1200,59 @@
       <c r="B41" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="9"/>
-      <c r="E41" s="10"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B42" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="D42" s="9"/>
-      <c r="E42" s="10"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B43" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="29"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="27"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B44" s="14" t="s">
         <v>44</v>
       </c>
       <c r="C44" s="9"/>
-      <c r="D44" s="11" t="s">
+      <c r="D44" s="21"/>
+      <c r="E44" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E44" s="10"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B45" s="14" t="s">
         <v>45</v>
       </c>
       <c r="C45" s="9"/>
-      <c r="D45" s="11" t="s">
+      <c r="D45" s="21"/>
+      <c r="E45" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="E45" s="10"/>
     </row>
     <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B46" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C46" s="24" t="s">
+      <c r="C46" s="29"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="D46" s="16"/>
-      <c r="E46" s="17"/>
     </row>
     <row r="47" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>